<commit_message>
Add P-ET-dS-RO / P
</commit_message>
<xml_diff>
--- a/tests/IHEWAdataanalysis/area1-GPM_MOD16A2_CSR.xlsx
+++ b/tests/IHEWAdataanalysis/area1-GPM_MOD16A2_CSR.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="63">
   <si>
     <t>date</t>
   </si>
@@ -152,9 +152,6 @@
     <t>Total Years</t>
   </si>
   <si>
-    <t>Diff %</t>
-  </si>
-  <si>
     <t>mean</t>
   </si>
   <si>
@@ -185,23 +182,38 @@
     <t>P-ET-dS (mm/year)</t>
   </si>
   <si>
-    <t>Diff % (from monthly)</t>
-  </si>
-  <si>
-    <t>Diff % (from yearly)</t>
-  </si>
-  <si>
     <t>Mm2</t>
   </si>
   <si>
     <t>years</t>
+  </si>
+  <si>
+    <t>Diff % over RO</t>
+  </si>
+  <si>
+    <t>Diff % over P</t>
+  </si>
+  <si>
+    <t>Diff % (from yearly) over RO</t>
+  </si>
+  <si>
+    <t>Diff % (from monthly) over RO</t>
+  </si>
+  <si>
+    <t>Diff % (from yearly) over P</t>
+  </si>
+  <si>
+    <t>Diff % (from monthly) over P</t>
+  </si>
+  <si>
+    <t>P (mm/year)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +232,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -251,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -262,8 +282,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -26443,68 +26464,72 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O97"/>
+  <dimension ref="A1:N97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
-        <v>49</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="4"/>
       <c r="G1" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>52</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>44</v>
+        <v>51</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1">
-        <v>21.503</v>
-      </c>
-      <c r="O1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>38353</v>
       </c>
@@ -26520,42 +26545,44 @@
         <f>C2/Runoff!B2</f>
         <v>-0.46252240291377128</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2">
+      <c r="E2" s="7">
+        <f>C2/GPM!I2</f>
+        <v>-0.29428085323789038</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2">
         <v>2005</v>
       </c>
-      <c r="G2">
+      <c r="H2">
+        <f>SUM(GPM!I2:I13)</f>
+        <v>2023.9859717358058</v>
+      </c>
+      <c r="I2">
         <f>SUM(B2:B13)</f>
         <v>844.214679035328</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <f>SUM(Runoff!B2:B13)</f>
         <v>612.5</v>
       </c>
-      <c r="I2">
-        <f>G2-H2</f>
+      <c r="K2">
+        <f>I2-J2</f>
         <v>231.714679035328</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <f>SUM(C2:C13)</f>
         <v>231.71467903532812</v>
       </c>
-      <c r="K2" s="7">
-        <f>J2/H2</f>
+      <c r="M2" s="7">
+        <f>L2/J2</f>
         <v>0.37830968005767857</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2" s="3">
-        <f>COUNTA(A2:A97)/12</f>
-        <v>8</v>
-      </c>
-      <c r="O2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N2" s="7">
+        <f>L2/H2</f>
+        <v>0.11448433055917159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>38384</v>
       </c>
@@ -26571,42 +26598,44 @@
         <f>C3/Runoff!B3</f>
         <v>-1.6467485164722484</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3">
+      <c r="E3" s="7">
+        <f>C3/GPM!I3</f>
+        <v>-1.4404857461141354</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3">
         <v>2006</v>
       </c>
-      <c r="G3">
+      <c r="H3">
+        <f>SUM(GPM!I14:I25)</f>
+        <v>2035.856086117092</v>
+      </c>
+      <c r="I3">
         <f>SUM(B14:B25)</f>
         <v>207.9320224521382</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <f>SUM(Runoff!B14:B25)</f>
         <v>747</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I9" si="0">G3-H3</f>
+      <c r="K3">
+        <f t="shared" ref="K3:K9" si="0">I3-J3</f>
         <v>-539.0679775478618</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <f>SUM(C14:C25)</f>
         <v>-539.06797754786169</v>
       </c>
-      <c r="K3" s="7">
-        <f t="shared" ref="K3:K9" si="1">J3/H3</f>
+      <c r="M3" s="7">
+        <f t="shared" ref="M3:M9" si="1">L3/J3</f>
         <v>-0.72164387891280013</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" s="8">
-        <f>SQRT(SUMSQ(C2:C97)/COUNTA(C2:C97))</f>
-        <v>110.21189909989434</v>
-      </c>
-      <c r="O3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N3" s="7">
+        <f t="shared" ref="N3:N9" si="2">L3/H3</f>
+        <v>-0.26478687821986707</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>38412</v>
       </c>
@@ -26622,42 +26651,44 @@
         <f>C4/Runoff!B4</f>
         <v>-0.77985778826312491</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4">
+      <c r="E4" s="7">
+        <f>C4/GPM!I4</f>
+        <v>-0.3532639764029471</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4">
         <v>2007</v>
       </c>
-      <c r="G4">
+      <c r="H4">
+        <f>SUM(GPM!I26:I37)</f>
+        <v>2029.9358274964065</v>
+      </c>
+      <c r="I4">
         <f>SUM(B26:B37)</f>
         <v>675.88940387632908</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <f>SUM(Runoff!B26:B37)</f>
         <v>735.49999999999989</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <f t="shared" si="0"/>
         <v>-59.610596123670803</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <f>SUM(C26:C37)</f>
         <v>-59.610596123670959</v>
       </c>
-      <c r="K4" s="7">
+      <c r="M4" s="7">
         <f t="shared" si="1"/>
         <v>-8.1047717367329658E-2</v>
       </c>
-      <c r="M4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="N4" s="8">
-        <f>SUM(C2:C97)/N2*N1</f>
-        <v>1009.7760469545499</v>
-      </c>
-      <c r="O4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N4" s="7">
+        <f t="shared" si="2"/>
+        <v>-2.9365753988977509E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>38443</v>
       </c>
@@ -26673,39 +26704,44 @@
         <f>C5/Runoff!B5</f>
         <v>-2.2599503891753985</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5">
+      <c r="E5" s="7">
+        <f>C5/GPM!I5</f>
+        <v>-2.0175061301956889</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5">
         <v>2008</v>
       </c>
-      <c r="G5">
+      <c r="H5">
+        <f>SUM(GPM!I38:I49)</f>
+        <v>2753.8990660919471</v>
+      </c>
+      <c r="I5">
         <f>SUM(B38:B49)</f>
         <v>1700.4054048904629</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <f>SUM(Runoff!B38:B49)</f>
         <v>1220.3</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <f t="shared" si="0"/>
         <v>480.10540489046298</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <f>SUM(C38:C49)</f>
         <v>480.10540489046286</v>
       </c>
-      <c r="K5" s="7">
+      <c r="M5" s="7">
         <f t="shared" si="1"/>
         <v>0.39343227476068415</v>
       </c>
-      <c r="M5" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="N5" s="9">
-        <f>AVERAGE(K2:K9)</f>
-        <v>1.5291422930469076E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N5" s="7">
+        <f t="shared" si="2"/>
+        <v>0.17433660180283206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>38473</v>
       </c>
@@ -26721,39 +26757,44 @@
         <f>C6/Runoff!B6</f>
         <v>-1.1928299351347535</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6">
+      <c r="E6" s="7">
+        <f>C6/GPM!I6</f>
+        <v>-0.13866005509969528</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6">
         <v>2009</v>
       </c>
-      <c r="G6">
+      <c r="H6">
+        <f>SUM(GPM!I50:I61)</f>
+        <v>2572.0574207525101</v>
+      </c>
+      <c r="I6">
         <f>SUM(B50:B61)</f>
         <v>1085.3783915866172</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <f>SUM(Runoff!B50:B61)</f>
         <v>1168.5999999999999</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <f t="shared" si="0"/>
         <v>-83.221608413382683</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <f>SUM(C50:C61)</f>
         <v>-83.221608413382825</v>
       </c>
-      <c r="K6" s="7">
+      <c r="M6" s="7">
         <f t="shared" si="1"/>
         <v>-7.1214794124065409E-2</v>
       </c>
-      <c r="M6" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="N6" s="7">
-        <f>AVERAGE(D2:D97)</f>
-        <v>2.6084512645679497E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>-3.2356046074987925E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>38504</v>
       </c>
@@ -26769,32 +26810,44 @@
         <f>C7/Runoff!B7</f>
         <v>1.6037676064730795</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7">
+      <c r="E7" s="7">
+        <f>C7/GPM!I7</f>
+        <v>0.38806228119503178</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7">
         <v>2010</v>
       </c>
-      <c r="G7">
+      <c r="H7">
+        <f>SUM(GPM!I62:I73)</f>
+        <v>2393.9888593300975</v>
+      </c>
+      <c r="I7">
         <f>SUM(B62:B73)</f>
         <v>541.19686117419451</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <f>SUM(Runoff!B62:B73)</f>
         <v>745.69999999999993</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <f t="shared" si="0"/>
         <v>-204.50313882580542</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <f>SUM(C62:C73)</f>
         <v>-204.50313882580542</v>
       </c>
-      <c r="K7" s="7">
+      <c r="M7" s="7">
         <f t="shared" si="1"/>
         <v>-0.27424317932922815</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N7" s="7">
+        <f t="shared" si="2"/>
+        <v>-8.5423596700876417E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>38534</v>
       </c>
@@ -26810,32 +26863,44 @@
         <f>C8/Runoff!B8</f>
         <v>1.8046818544857353</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8">
+      <c r="E8" s="7">
+        <f>C8/GPM!I8</f>
+        <v>0.47635089621007548</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8">
         <v>2011</v>
       </c>
-      <c r="G8">
+      <c r="H8">
+        <f>SUM(GPM!I74:I85)</f>
+        <v>2710.3295393318917</v>
+      </c>
+      <c r="I8">
         <f>SUM(B74:B85)</f>
         <v>1529.5837447607494</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <f>SUM(Runoff!B74:B85)</f>
         <v>1086.9999999999998</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <f t="shared" si="0"/>
         <v>442.5837447607496</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <f>SUM(C74:C85)</f>
         <v>442.58374476074948</v>
       </c>
-      <c r="K8" s="7">
+      <c r="M8" s="7">
         <f t="shared" si="1"/>
         <v>0.40716075874953961</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N8" s="7">
+        <f t="shared" si="2"/>
+        <v>0.16329517807264438</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>38565</v>
       </c>
@@ -26851,32 +26916,44 @@
         <f>C9/Runoff!B9</f>
         <v>2.5179430128682174</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9">
+      <c r="E9" s="7">
+        <f>C9/GPM!I9</f>
+        <v>0.56978837471743349</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9">
         <v>2012</v>
       </c>
-      <c r="G9">
+      <c r="H9">
+        <f>SUM(GPM!I86:I97)</f>
+        <v>2315.2674883261429</v>
+      </c>
+      <c r="I9">
         <f>SUM(B86:B97)</f>
         <v>1283.4776941325842</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <f>SUM(Runoff!B86:B97)</f>
         <v>1175.8000000000002</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <f t="shared" si="0"/>
         <v>107.67769413258407</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <f>SUM(C86:C97)</f>
         <v>107.67769413258395</v>
       </c>
-      <c r="K9" s="7">
+      <c r="M9" s="7">
         <f t="shared" si="1"/>
         <v>9.1578239609273637E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N9" s="7">
+        <f t="shared" si="2"/>
+        <v>4.6507669060058002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>38596</v>
       </c>
@@ -26892,32 +26969,44 @@
         <f>C10/Runoff!B10</f>
         <v>1.5746808061983688</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10">
-        <f>AVERAGE(G2:G9)</f>
-        <v>983.50977523855045</v>
+      <c r="E10" s="7">
+        <f>C10/GPM!I10</f>
+        <v>0.44627408576249034</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="H10">
         <f>AVERAGE(H2:H9)</f>
-        <v>936.55</v>
+        <v>2354.4150323977365</v>
       </c>
       <c r="I10">
         <f>AVERAGE(I2:I9)</f>
-        <v>46.959775238550492</v>
+        <v>983.50977523855045</v>
       </c>
       <c r="J10">
         <f>AVERAGE(J2:J9)</f>
+        <v>936.55</v>
+      </c>
+      <c r="K10">
+        <f>AVERAGE(K2:K9)</f>
+        <v>46.959775238550492</v>
+      </c>
+      <c r="L10">
+        <f>AVERAGE(L2:L9)</f>
         <v>46.959775238550435</v>
       </c>
-      <c r="K10" s="7">
-        <f>AVERAGE(K2:K9)</f>
+      <c r="M10" s="7">
+        <f>AVERAGE(M2:M9)</f>
         <v>1.5291422930469076E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N10" s="7">
+        <f>AVERAGE(N2:N9)</f>
+        <v>1.083643806374964E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>38626</v>
       </c>
@@ -26933,9 +27022,13 @@
         <f>C11/Runoff!B11</f>
         <v>0.55193577621448142</v>
       </c>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E11" s="7">
+        <f>C11/GPM!I11</f>
+        <v>0.12871905925002597</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>38657</v>
       </c>
@@ -26951,9 +27044,13 @@
         <f>C12/Runoff!B12</f>
         <v>-2.7681773245514161</v>
       </c>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E12" s="7">
+        <f>C12/GPM!I12</f>
+        <v>-1.2583926176811082</v>
+      </c>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>38687</v>
       </c>
@@ -26969,9 +27066,13 @@
         <f>C13/Runoff!B13</f>
         <v>3.6551939325921192</v>
       </c>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E13" s="7">
+        <f>C13/GPM!I13</f>
+        <v>0.72437009858114132</v>
+      </c>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>38718</v>
       </c>
@@ -26987,9 +27088,22 @@
         <f>C14/Runoff!B14</f>
         <v>-2.2384619926540594</v>
       </c>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E14" s="7">
+        <f>C14/GPM!I14</f>
+        <v>-1.2634495686592309</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14">
+        <v>21.503</v>
+      </c>
+      <c r="I14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>38749</v>
       </c>
@@ -27005,9 +27119,23 @@
         <f>C15/Runoff!B15</f>
         <v>1.1761318125014273</v>
       </c>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E15" s="7">
+        <f>C15/GPM!I15</f>
+        <v>0.3973515408403312</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="3">
+        <f>COUNTA(A2:A97)/12</f>
+        <v>8</v>
+      </c>
+      <c r="I15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>38777</v>
       </c>
@@ -27023,9 +27151,23 @@
         <f>C16/Runoff!B16</f>
         <v>-0.11965858464934501</v>
       </c>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="7">
+        <f>C16/GPM!I16</f>
+        <v>-5.0479746732310392E-2</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="9">
+        <f>SQRT(SUMSQ(C2:C97)/COUNTA(C2:C97))</f>
+        <v>110.21189909989434</v>
+      </c>
+      <c r="I16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>38808</v>
       </c>
@@ -27041,9 +27183,23 @@
         <f>C17/Runoff!B17</f>
         <v>-1.9909460070004339</v>
       </c>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="7">
+        <f>C17/GPM!I17</f>
+        <v>-0.89537174580905954</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="9">
+        <f>SUM(C2:C97)/H15*H14</f>
+        <v>1009.7760469545499</v>
+      </c>
+      <c r="I17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>38838</v>
       </c>
@@ -27059,9 +27215,20 @@
         <f>C18/Runoff!B18</f>
         <v>-6.8094166009337185</v>
       </c>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="7">
+        <f>C18/GPM!I18</f>
+        <v>-2.1188027866116972</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="8">
+        <f>AVERAGE(M2:M9)</f>
+        <v>1.5291422930469076E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>38869</v>
       </c>
@@ -27077,9 +27244,20 @@
         <f>C19/Runoff!B19</f>
         <v>4.2856329729754048</v>
       </c>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="7">
+        <f>C19/GPM!I19</f>
+        <v>0.65248387015811937</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" s="7">
+        <f>AVERAGE(D2:D97)</f>
+        <v>2.6084512645679497E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>38899</v>
       </c>
@@ -27095,9 +27273,20 @@
         <f>C20/Runoff!B20</f>
         <v>0.35542709497353303</v>
       </c>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="7">
+        <f>C20/GPM!I20</f>
+        <v>0.19178033035725497</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" s="10">
+        <f>AVERAGE(N2:N9)</f>
+        <v>1.083643806374964E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>38930</v>
       </c>
@@ -27113,9 +27302,20 @@
         <f>C21/Runoff!B21</f>
         <v>1.5610204011846618</v>
       </c>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="7">
+        <f>C21/GPM!I21</f>
+        <v>0.46248727693619257</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="7">
+        <f>AVERAGE(E2:E97)</f>
+        <v>-0.12556242059636039</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>38961</v>
       </c>
@@ -27131,9 +27331,13 @@
         <f>C22/Runoff!B22</f>
         <v>0.61942001694848459</v>
       </c>
-      <c r="E22" s="7"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="7">
+        <f>C22/GPM!I22</f>
+        <v>0.18626249854960658</v>
+      </c>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>38991</v>
       </c>
@@ -27149,9 +27353,13 @@
         <f>C23/Runoff!B23</f>
         <v>0.98410354332749517</v>
       </c>
-      <c r="E23" s="7"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="7">
+        <f>C23/GPM!I23</f>
+        <v>0.25538517002216443</v>
+      </c>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>39022</v>
       </c>
@@ -27167,9 +27375,13 @@
         <f>C24/Runoff!B24</f>
         <v>-4.0825873969930973</v>
       </c>
-      <c r="E24" s="7"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="7">
+        <f>C24/GPM!I24</f>
+        <v>-2.3318984343187021</v>
+      </c>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>39052</v>
       </c>
@@ -27185,9 +27397,13 @@
         <f>C25/Runoff!B25</f>
         <v>-0.36498235975433663</v>
       </c>
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="7">
+        <f>C25/GPM!I25</f>
+        <v>-0.25249194887705756</v>
+      </c>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>39083</v>
       </c>
@@ -27203,9 +27419,13 @@
         <f>C26/Runoff!B26</f>
         <v>0.93048959643384466</v>
       </c>
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="7">
+        <f>C26/GPM!I26</f>
+        <v>0.28609766649352852</v>
+      </c>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>39114</v>
       </c>
@@ -27221,9 +27441,13 @@
         <f>C27/Runoff!B27</f>
         <v>-0.85458335555608644</v>
       </c>
-      <c r="E27" s="7"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="7">
+        <f>C27/GPM!I27</f>
+        <v>-0.66279777499092341</v>
+      </c>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>39142</v>
       </c>
@@ -27239,9 +27463,13 @@
         <f>C28/Runoff!B28</f>
         <v>-2.0534693317012236</v>
       </c>
-      <c r="E28" s="7"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="7">
+        <f>C28/GPM!I28</f>
+        <v>-1.6189918549129636</v>
+      </c>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>39173</v>
       </c>
@@ -27257,9 +27485,13 @@
         <f>C29/Runoff!B29</f>
         <v>-2.1340087689149567</v>
       </c>
-      <c r="E29" s="7"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="7">
+        <f>C29/GPM!I29</f>
+        <v>-1.0555821814345945</v>
+      </c>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>39203</v>
       </c>
@@ -27275,9 +27507,13 @@
         <f>C30/Runoff!B30</f>
         <v>-2.4698387158232507</v>
       </c>
-      <c r="E30" s="7"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="7">
+        <f>C30/GPM!I30</f>
+        <v>-0.57861494126377044</v>
+      </c>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>39234</v>
       </c>
@@ -27293,9 +27529,13 @@
         <f>C31/Runoff!B31</f>
         <v>4.2360656755896979</v>
       </c>
-      <c r="E31" s="7"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="7">
+        <f>C31/GPM!I31</f>
+        <v>0.58737488492202783</v>
+      </c>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>39264</v>
       </c>
@@ -27311,9 +27551,13 @@
         <f>C32/Runoff!B32</f>
         <v>1.121317149296909</v>
       </c>
-      <c r="E32" s="7"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="7">
+        <f>C32/GPM!I32</f>
+        <v>0.34920748720944933</v>
+      </c>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>39295</v>
       </c>
@@ -27329,9 +27573,13 @@
         <f>C33/Runoff!B33</f>
         <v>1.8695301807316853</v>
       </c>
-      <c r="E33" s="7"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="7">
+        <f>C33/GPM!I33</f>
+        <v>0.49644605986063972</v>
+      </c>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>39326</v>
       </c>
@@ -27347,9 +27595,13 @@
         <f>C34/Runoff!B34</f>
         <v>7.9058634553036841E-2</v>
       </c>
-      <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="7">
+        <f>C34/GPM!I34</f>
+        <v>4.0623496295989943E-2</v>
+      </c>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>39356</v>
       </c>
@@ -27365,9 +27617,13 @@
         <f>C35/Runoff!B35</f>
         <v>-0.2990185155304349</v>
       </c>
-      <c r="E35" s="7"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="7">
+        <f>C35/GPM!I35</f>
+        <v>-9.9882673412818881E-2</v>
+      </c>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>39387</v>
       </c>
@@ -27383,9 +27639,13 @@
         <f>C36/Runoff!B36</f>
         <v>-1.2121547876603467</v>
       </c>
-      <c r="E36" s="7"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="7">
+        <f>C36/GPM!I36</f>
+        <v>-0.43731562803318808</v>
+      </c>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>39417</v>
       </c>
@@ -27401,9 +27661,13 @@
         <f>C37/Runoff!B37</f>
         <v>0.16489912259690881</v>
       </c>
-      <c r="E37" s="7"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="7">
+        <f>C37/GPM!I37</f>
+        <v>9.6876254564241676E-2</v>
+      </c>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>39448</v>
       </c>
@@ -27419,9 +27683,13 @@
         <f>C38/Runoff!B38</f>
         <v>-8.1844401049347024E-2</v>
       </c>
-      <c r="E38" s="7"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="7">
+        <f>C38/GPM!I38</f>
+        <v>-3.7131816214134826E-2</v>
+      </c>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>39479</v>
       </c>
@@ -27437,9 +27705,13 @@
         <f>C39/Runoff!B39</f>
         <v>0.99073424214450601</v>
       </c>
-      <c r="E39" s="7"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="7">
+        <f>C39/GPM!I39</f>
+        <v>0.35138882816253342</v>
+      </c>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39508</v>
       </c>
@@ -27455,9 +27727,13 @@
         <f>C40/Runoff!B40</f>
         <v>1.1890842229749168</v>
       </c>
-      <c r="E40" s="7"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="7">
+        <f>C40/GPM!I40</f>
+        <v>0.42403457732136379</v>
+      </c>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39539</v>
       </c>
@@ -27473,9 +27749,13 @@
         <f>C41/Runoff!B41</f>
         <v>0.96238612193163864</v>
       </c>
-      <c r="E41" s="7"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="7">
+        <f>C41/GPM!I41</f>
+        <v>0.35768622983102766</v>
+      </c>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>39569</v>
       </c>
@@ -27491,9 +27771,13 @@
         <f>C42/Runoff!B42</f>
         <v>1.3030020549136421</v>
       </c>
-      <c r="E42" s="7"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="7">
+        <f>C42/GPM!I42</f>
+        <v>0.30200998735860352</v>
+      </c>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>39600</v>
       </c>
@@ -27509,9 +27793,13 @@
         <f>C43/Runoff!B43</f>
         <v>0.29979990081847024</v>
       </c>
-      <c r="E43" s="7"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E43" s="7">
+        <f>C43/GPM!I43</f>
+        <v>7.4402645681442614E-2</v>
+      </c>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>39630</v>
       </c>
@@ -27527,9 +27815,13 @@
         <f>C44/Runoff!B44</f>
         <v>-0.10804580783098179</v>
       </c>
-      <c r="E44" s="7"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E44" s="7">
+        <f>C44/GPM!I44</f>
+        <v>-8.3286220054097512E-2</v>
+      </c>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>39661</v>
       </c>
@@ -27545,9 +27837,13 @@
         <f>C45/Runoff!B45</f>
         <v>0.4308129529526144</v>
       </c>
-      <c r="E45" s="7"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E45" s="7">
+        <f>C45/GPM!I45</f>
+        <v>0.23169772732581656</v>
+      </c>
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>39692</v>
       </c>
@@ -27563,9 +27859,13 @@
         <f>C46/Runoff!B46</f>
         <v>0.83880921542452969</v>
       </c>
-      <c r="E46" s="7"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E46" s="7">
+        <f>C46/GPM!I46</f>
+        <v>0.39801594985106581</v>
+      </c>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>39722</v>
       </c>
@@ -27581,9 +27881,13 @@
         <f>C47/Runoff!B47</f>
         <v>-8.5397728791896263E-2</v>
       </c>
-      <c r="E47" s="7"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E47" s="7">
+        <f>C47/GPM!I47</f>
+        <v>-4.6935204346710606E-2</v>
+      </c>
+      <c r="F47" s="7"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>39753</v>
       </c>
@@ -27599,9 +27903,13 @@
         <f>C48/Runoff!B48</f>
         <v>0.13626545545221674</v>
       </c>
-      <c r="E48" s="7"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E48" s="7">
+        <f>C48/GPM!I48</f>
+        <v>6.1958977256879946E-2</v>
+      </c>
+      <c r="F48" s="7"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>39783</v>
       </c>
@@ -27617,9 +27925,13 @@
         <f>C49/Runoff!B49</f>
         <v>7.6339805915827848E-3</v>
       </c>
-      <c r="E49" s="7"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E49" s="7">
+        <f>C49/GPM!I49</f>
+        <v>5.9033546410142855E-3</v>
+      </c>
+      <c r="F49" s="7"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>39814</v>
       </c>
@@ -27635,9 +27947,13 @@
         <f>C50/Runoff!B50</f>
         <v>2.3762155794089284E-2</v>
       </c>
-      <c r="E50" s="7"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E50" s="7">
+        <f>C50/GPM!I50</f>
+        <v>9.7646753747502348E-3</v>
+      </c>
+      <c r="F50" s="7"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>39845</v>
       </c>
@@ -27653,9 +27969,13 @@
         <f>C51/Runoff!B51</f>
         <v>0.57853110647556916</v>
       </c>
-      <c r="E51" s="7"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E51" s="7">
+        <f>C51/GPM!I51</f>
+        <v>0.32278708163995595</v>
+      </c>
+      <c r="F51" s="7"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>39873</v>
       </c>
@@ -27671,9 +27991,13 @@
         <f>C52/Runoff!B52</f>
         <v>-0.54210620420530486</v>
       </c>
-      <c r="E52" s="7"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E52" s="7">
+        <f>C52/GPM!I52</f>
+        <v>-0.39946054078043697</v>
+      </c>
+      <c r="F52" s="7"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>39904</v>
       </c>
@@ -27689,9 +28013,13 @@
         <f>C53/Runoff!B53</f>
         <v>1.2776456131371325</v>
       </c>
-      <c r="E53" s="7"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E53" s="7">
+        <f>C53/GPM!I53</f>
+        <v>0.33337310899988626</v>
+      </c>
+      <c r="F53" s="7"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>39934</v>
       </c>
@@ -27707,9 +28035,13 @@
         <f>C54/Runoff!B54</f>
         <v>-0.99626914251383769</v>
       </c>
-      <c r="E54" s="7"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E54" s="7">
+        <f>C54/GPM!I54</f>
+        <v>-0.29466744570210329</v>
+      </c>
+      <c r="F54" s="7"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>39965</v>
       </c>
@@ -27725,9 +28057,13 @@
         <f>C55/Runoff!B55</f>
         <v>0.47131118140530853</v>
       </c>
-      <c r="E55" s="7"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E55" s="7">
+        <f>C55/GPM!I55</f>
+        <v>0.23012544132989995</v>
+      </c>
+      <c r="F55" s="7"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>39995</v>
       </c>
@@ -27743,9 +28079,13 @@
         <f>C56/Runoff!B56</f>
         <v>2.4703180797760784</v>
       </c>
-      <c r="E56" s="7"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E56" s="7">
+        <f>C56/GPM!I56</f>
+        <v>0.63391920581117089</v>
+      </c>
+      <c r="F56" s="7"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>40026</v>
       </c>
@@ -27761,9 +28101,13 @@
         <f>C57/Runoff!B57</f>
         <v>3.2296170768745026E-3</v>
       </c>
-      <c r="E57" s="7"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E57" s="7">
+        <f>C57/GPM!I57</f>
+        <v>2.1345714094947459E-3</v>
+      </c>
+      <c r="F57" s="7"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>40057</v>
       </c>
@@ -27779,9 +28123,13 @@
         <f>C58/Runoff!B58</f>
         <v>0.98119907015332564</v>
       </c>
-      <c r="E58" s="7"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E58" s="7">
+        <f>C58/GPM!I58</f>
+        <v>0.40870843305289861</v>
+      </c>
+      <c r="F58" s="7"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>40087</v>
       </c>
@@ -27797,9 +28145,13 @@
         <f>C59/Runoff!B59</f>
         <v>-1.2266737248397142</v>
       </c>
-      <c r="E59" s="7"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E59" s="7">
+        <f>C59/GPM!I59</f>
+        <v>-0.89524711820161329</v>
+      </c>
+      <c r="F59" s="7"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>40118</v>
       </c>
@@ -27815,9 +28167,13 @@
         <f>C60/Runoff!B60</f>
         <v>-3.2423553498688418</v>
       </c>
-      <c r="E60" s="7"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E60" s="7">
+        <f>C60/GPM!I60</f>
+        <v>-1.4199777914225367</v>
+      </c>
+      <c r="F60" s="7"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>40148</v>
       </c>
@@ -27833,9 +28189,13 @@
         <f>C61/Runoff!B61</f>
         <v>-0.65660124184752511</v>
       </c>
-      <c r="E61" s="7"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E61" s="7">
+        <f>C61/GPM!I61</f>
+        <v>-0.81119947843626816</v>
+      </c>
+      <c r="F61" s="7"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>40179</v>
       </c>
@@ -27851,9 +28211,13 @@
         <f>C62/Runoff!B62</f>
         <v>-4.4591786208701487</v>
       </c>
-      <c r="E62" s="7"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E62" s="7">
+        <f>C62/GPM!I62</f>
+        <v>-1.4791743377844937</v>
+      </c>
+      <c r="F62" s="7"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>40210</v>
       </c>
@@ -27869,9 +28233,13 @@
         <f>C63/Runoff!B63</f>
         <v>-1.3326690489848052</v>
       </c>
-      <c r="E63" s="7"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E63" s="7">
+        <f>C63/GPM!I63</f>
+        <v>-1.0475266068432867</v>
+      </c>
+      <c r="F63" s="7"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>40238</v>
       </c>
@@ -27887,9 +28255,13 @@
         <f>C64/Runoff!B64</f>
         <v>-2.0650831953096671</v>
       </c>
-      <c r="E64" s="7"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E64" s="7">
+        <f>C64/GPM!I64</f>
+        <v>-1.5243437315170347</v>
+      </c>
+      <c r="F64" s="7"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>40269</v>
       </c>
@@ -27905,9 +28277,13 @@
         <f>C65/Runoff!B65</f>
         <v>-2.5083498966640603</v>
       </c>
-      <c r="E65" s="7"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E65" s="7">
+        <f>C65/GPM!I65</f>
+        <v>-0.54753447291350821</v>
+      </c>
+      <c r="F65" s="7"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>40299</v>
       </c>
@@ -27923,9 +28299,13 @@
         <f>C66/Runoff!B66</f>
         <v>-2.04308101593096</v>
       </c>
-      <c r="E66" s="7"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E66" s="7">
+        <f>C66/GPM!I66</f>
+        <v>-0.22939620154856172</v>
+      </c>
+      <c r="F66" s="7"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>40330</v>
       </c>
@@ -27941,9 +28321,13 @@
         <f>C67/Runoff!B67</f>
         <v>1.5455772304821689</v>
       </c>
-      <c r="E67" s="7"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="7">
+        <f>C67/GPM!I67</f>
+        <v>0.42142273861790841</v>
+      </c>
+      <c r="F67" s="7"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>40360</v>
       </c>
@@ -27959,9 +28343,13 @@
         <f>C68/Runoff!B68</f>
         <v>2.931039767877325</v>
       </c>
-      <c r="E68" s="7"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E68" s="7">
+        <f>C68/GPM!I68</f>
+        <v>0.55737492329350546</v>
+      </c>
+      <c r="F68" s="7"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>40391</v>
       </c>
@@ -27977,9 +28365,13 @@
         <f>C69/Runoff!B69</f>
         <v>0.91122444045658724</v>
       </c>
-      <c r="E69" s="7"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E69" s="7">
+        <f>C69/GPM!I69</f>
+        <v>0.34492732635921197</v>
+      </c>
+      <c r="F69" s="7"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>40422</v>
       </c>
@@ -27995,9 +28387,13 @@
         <f>C70/Runoff!B70</f>
         <v>0.68413081212395532</v>
       </c>
-      <c r="E70" s="7"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E70" s="7">
+        <f>C70/GPM!I70</f>
+        <v>0.20429967878025954</v>
+      </c>
+      <c r="F70" s="7"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>40452</v>
       </c>
@@ -28013,9 +28409,13 @@
         <f>C71/Runoff!B71</f>
         <v>0.37647480555220864</v>
       </c>
-      <c r="E71" s="7"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="7">
+        <f>C71/GPM!I71</f>
+        <v>0.10703105731937618</v>
+      </c>
+      <c r="F71" s="7"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>40483</v>
       </c>
@@ -28031,9 +28431,13 @@
         <f>C72/Runoff!B72</f>
         <v>-1.6626631736123965</v>
       </c>
-      <c r="E72" s="7"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E72" s="7">
+        <f>C72/GPM!I72</f>
+        <v>-0.76290615452425481</v>
+      </c>
+      <c r="F72" s="7"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>40513</v>
       </c>
@@ -28049,9 +28453,13 @@
         <f>C73/Runoff!B73</f>
         <v>1.3834086700080264</v>
       </c>
-      <c r="E73" s="7"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E73" s="7">
+        <f>C73/GPM!I73</f>
+        <v>0.4690804919256944</v>
+      </c>
+      <c r="F73" s="7"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>40544</v>
       </c>
@@ -28067,9 +28475,13 @@
         <f>C74/Runoff!B74</f>
         <v>-0.20072560575262985</v>
       </c>
-      <c r="E74" s="7"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E74" s="7">
+        <f>C74/GPM!I74</f>
+        <v>-4.9520091946968527E-2</v>
+      </c>
+      <c r="F74" s="7"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>40575</v>
       </c>
@@ -28085,9 +28497,13 @@
         <f>C75/Runoff!B75</f>
         <v>1.7274233027171704</v>
       </c>
-      <c r="E75" s="7"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E75" s="7">
+        <f>C75/GPM!I75</f>
+        <v>0.43619692491534628</v>
+      </c>
+      <c r="F75" s="7"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>40603</v>
       </c>
@@ -28103,9 +28519,13 @@
         <f>C76/Runoff!B76</f>
         <v>1.069167796364878</v>
       </c>
-      <c r="E76" s="7"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E76" s="7">
+        <f>C76/GPM!I76</f>
+        <v>0.35392051806229563</v>
+      </c>
+      <c r="F76" s="7"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>40634</v>
       </c>
@@ -28121,9 +28541,13 @@
         <f>C77/Runoff!B77</f>
         <v>-0.70559243746127853</v>
       </c>
-      <c r="E77" s="7"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E77" s="7">
+        <f>C77/GPM!I77</f>
+        <v>-0.32172155780142714</v>
+      </c>
+      <c r="F77" s="7"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>40664</v>
       </c>
@@ -28139,9 +28563,13 @@
         <f>C78/Runoff!B78</f>
         <v>2.6028167545177312</v>
       </c>
-      <c r="E78" s="7"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E78" s="7">
+        <f>C78/GPM!I78</f>
+        <v>0.53289097478578928</v>
+      </c>
+      <c r="F78" s="7"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>40695</v>
       </c>
@@ -28157,9 +28585,13 @@
         <f>C79/Runoff!B79</f>
         <v>1.2364413066009199</v>
       </c>
-      <c r="E79" s="7"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E79" s="7">
+        <f>C79/GPM!I79</f>
+        <v>0.47440022547358529</v>
+      </c>
+      <c r="F79" s="7"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>40725</v>
       </c>
@@ -28175,9 +28607,13 @@
         <f>C80/Runoff!B80</f>
         <v>0.5945943858855236</v>
       </c>
-      <c r="E80" s="7"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E80" s="7">
+        <f>C80/GPM!I80</f>
+        <v>0.2825239378930931</v>
+      </c>
+      <c r="F80" s="7"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>40756</v>
       </c>
@@ -28193,9 +28629,13 @@
         <f>C81/Runoff!B81</f>
         <v>1.3776779524007698</v>
       </c>
-      <c r="E81" s="7"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E81" s="7">
+        <f>C81/GPM!I81</f>
+        <v>0.42692792403618196</v>
+      </c>
+      <c r="F81" s="7"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>40787</v>
       </c>
@@ -28211,9 +28651,13 @@
         <f>C82/Runoff!B82</f>
         <v>0.56767568786196765</v>
       </c>
-      <c r="E82" s="7"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E82" s="7">
+        <f>C82/GPM!I82</f>
+        <v>0.27388836231548497</v>
+      </c>
+      <c r="F82" s="7"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>40817</v>
       </c>
@@ -28229,9 +28673,13 @@
         <f>C83/Runoff!B83</f>
         <v>-0.21851013397570596</v>
       </c>
-      <c r="E83" s="7"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E83" s="7">
+        <f>C83/GPM!I83</f>
+        <v>-0.14108077556691889</v>
+      </c>
+      <c r="F83" s="7"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>40848</v>
       </c>
@@ -28247,9 +28695,13 @@
         <f>C84/Runoff!B84</f>
         <v>-1.3765617897415181</v>
       </c>
-      <c r="E84" s="7"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E84" s="7">
+        <f>C84/GPM!I84</f>
+        <v>-0.76648913397683283</v>
+      </c>
+      <c r="F84" s="7"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>40878</v>
       </c>
@@ -28265,9 +28717,13 @@
         <f>C85/Runoff!B85</f>
         <v>0.15697239372230351</v>
       </c>
-      <c r="E85" s="7"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E85" s="7">
+        <f>C85/GPM!I85</f>
+        <v>9.0561977095757556E-2</v>
+      </c>
+      <c r="F85" s="7"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>40909</v>
       </c>
@@ -28283,9 +28739,13 @@
         <f>C86/Runoff!B86</f>
         <v>-0.74341556717196555</v>
       </c>
-      <c r="E86" s="7"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E86" s="7">
+        <f>C86/GPM!I86</f>
+        <v>-0.58646550688603138</v>
+      </c>
+      <c r="F86" s="7"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>40940</v>
       </c>
@@ -28301,9 +28761,13 @@
         <f>C87/Runoff!B87</f>
         <v>0.85621715613794414</v>
       </c>
-      <c r="E87" s="7"/>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E87" s="7">
+        <f>C87/GPM!I87</f>
+        <v>0.38984446578986337</v>
+      </c>
+      <c r="F87" s="7"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>40969</v>
       </c>
@@ -28319,9 +28783,13 @@
         <f>C88/Runoff!B88</f>
         <v>2.9918533877076423E-2</v>
       </c>
-      <c r="E88" s="7"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E88" s="7">
+        <f>C88/GPM!I88</f>
+        <v>2.3759933448535584E-2</v>
+      </c>
+      <c r="F88" s="7"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>41000</v>
       </c>
@@ -28337,9 +28805,13 @@
         <f>C89/Runoff!B89</f>
         <v>0.13680441002000274</v>
       </c>
-      <c r="E89" s="7"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E89" s="7">
+        <f>C89/GPM!I89</f>
+        <v>6.4191178564233412E-2</v>
+      </c>
+      <c r="F89" s="7"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>41030</v>
       </c>
@@ -28355,9 +28827,13 @@
         <f>C90/Runoff!B90</f>
         <v>0.27217230092320277</v>
       </c>
-      <c r="E90" s="7"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E90" s="7">
+        <f>C90/GPM!I90</f>
+        <v>8.2642435086794364E-2</v>
+      </c>
+      <c r="F90" s="7"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>41061</v>
       </c>
@@ -28373,9 +28849,13 @@
         <f>C91/Runoff!B91</f>
         <v>-1.4659750351871956</v>
       </c>
-      <c r="E91" s="7"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E91" s="7">
+        <f>C91/GPM!I91</f>
+        <v>-0.76395664053333778</v>
+      </c>
+      <c r="F91" s="7"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>41091</v>
       </c>
@@ -28391,9 +28871,13 @@
         <f>C92/Runoff!B92</f>
         <v>1.5466342207393067</v>
       </c>
-      <c r="E92" s="7"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E92" s="7">
+        <f>C92/GPM!I92</f>
+        <v>0.50835302897584667</v>
+      </c>
+      <c r="F92" s="7"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>41122</v>
       </c>
@@ -28409,9 +28893,13 @@
         <f>C93/Runoff!B93</f>
         <v>0.67256251004800238</v>
       </c>
-      <c r="E93" s="7"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E93" s="7">
+        <f>C93/GPM!I93</f>
+        <v>0.34551555910169562</v>
+      </c>
+      <c r="F93" s="7"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>41153</v>
       </c>
@@ -28427,9 +28915,13 @@
         <f>C94/Runoff!B94</f>
         <v>1.0158262919354373</v>
       </c>
-      <c r="E94" s="7"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E94" s="7">
+        <f>C94/GPM!I94</f>
+        <v>0.43302513757694133</v>
+      </c>
+      <c r="F94" s="7"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>41183</v>
       </c>
@@ -28445,9 +28937,13 @@
         <f>C95/Runoff!B95</f>
         <v>0.77267612489907311</v>
       </c>
-      <c r="E95" s="7"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E95" s="7">
+        <f>C95/GPM!I95</f>
+        <v>0.35255040702955714</v>
+      </c>
+      <c r="F95" s="7"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>41214</v>
       </c>
@@ -28463,9 +28959,13 @@
         <f>C96/Runoff!B96</f>
         <v>-1.2940718988952153</v>
       </c>
-      <c r="E96" s="7"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E96" s="7">
+        <f>C96/GPM!I96</f>
+        <v>-0.84002704519254356</v>
+      </c>
+      <c r="F96" s="7"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>41244</v>
       </c>
@@ -28481,13 +28981,17 @@
         <f>C97/Runoff!B97</f>
         <v>-0.26476400794693661</v>
       </c>
-      <c r="E97" s="7"/>
+      <c r="E97" s="7">
+        <f>C97/GPM!I97</f>
+        <v>-0.19685717469022157</v>
+      </c>
+      <c r="F97" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="H2:H10" formulaRange="1"/>
+    <ignoredError sqref="J2:J10 H2:H9" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>